<commit_message>
added response for excel
</commit_message>
<xml_diff>
--- a/server/internship_records.xlsx
+++ b/server/internship_records.xlsx
@@ -397,86 +397,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>acad_year</v>
+        <v>curriculum</v>
       </c>
       <c r="B1" t="str">
+        <v>english_name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>placement_id</v>
+      </c>
+      <c r="D1" t="str">
         <v>placement_year</v>
+      </c>
+      <c r="E1" t="str">
+        <v>company_name</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2021</v>
+        <v>BBA(IS)</v>
       </c>
       <c r="B2" t="str">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B8" t="str">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>2021</v>
-      </c>
-      <c r="B9" t="str">
+        <v>Bob Doe</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="str">
         <v>2022</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>